<commit_message>
Url_List.xlsx has been updated
</commit_message>
<xml_diff>
--- a/Url_List.xlsx
+++ b/Url_List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://163gc-my.sharepoint.com/personal/abdelmonaam_kallali_ssc-spc_gc_ca/Documents/Documents/App-Monitor/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://163gc-my.sharepoint.com/personal/abdelmonaam_kallali_ssc-spc_gc_ca/Documents/Documents/ProdApplicationMonitoring/ProdApplicationMonitoring/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="114_{E30C56CB-0642-486D-B1FB-CBD893529A96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="114_{E30C56CB-0642-486D-B1FB-CBD893529A96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0D26CF6E-7F60-F541-A4C8-FB127C80CFE9}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D13659F6-ED47-4C0E-9560-3CD668E37EED}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{D13659F6-ED47-4C0E-9560-3CD668E37EED}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -112,9 +112,6 @@
     <t>chiranjeev.kumar@ssc-spc.gc.ca,CIOApplicationSupport-DPISupportdApplications@ssc-spc.gc.ca</t>
   </si>
   <si>
-    <t>mikael.levesque@ssc-spc.gc.ca,muhes.ariyaratnam@ssc-spc.gc.ca,archermanagement-gestiondearcher@ssc-spc.gc.ca</t>
-  </si>
-  <si>
     <t>albert.saikaley@ssc-spc.gc.ca,chiranjeev.kumar@ssc-spc.gc.ca,CIOApplicationSupport-DPISupportdApplications@ssc-spc.gc.ca</t>
   </si>
   <si>
@@ -146,6 +143,9 @@
   </si>
   <si>
     <t>abdelmonaam.kallali@ssc-spc.gc.ca,simon.lowe@ssc-spc.gc.ca,servicenowcio-servicenowdpi@ssc-spc.gc.ca</t>
+  </si>
+  <si>
+    <t>abdelmonaam.kallali@ssc-spc.gc.ca,abdellah.arba@ssc-spc.gc.ca,archermanagement-gestiondearcher@ssc-spc.gc.ca</t>
   </si>
 </sst>
 </file>
@@ -560,18 +560,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A17F301F-A4BC-4FEF-A93E-385FAF2DEAD9}">
   <dimension ref="B1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="72.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.5546875" customWidth="1"/>
-    <col min="4" max="4" width="33.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="72.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.5" customWidth="1"/>
+    <col min="4" max="4" width="33.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -582,7 +582,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>10</v>
       </c>
@@ -590,10 +590,10 @@
         <v>3</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
         <v>9</v>
       </c>
@@ -601,10 +601,10 @@
         <v>4</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B4" s="3" t="s">
         <v>12</v>
       </c>
@@ -612,10 +612,10 @@
         <v>11</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
@@ -623,10 +623,10 @@
         <v>5</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
         <v>6</v>
       </c>
@@ -637,29 +637,29 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
         <v>30</v>
-      </c>
-      <c r="C8" t="s">
-        <v>31</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B9" s="3" t="s">
         <v>20</v>
       </c>
@@ -670,7 +670,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B10" s="3" t="s">
         <v>14</v>
       </c>
@@ -681,7 +681,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B11" s="3" t="s">
         <v>21</v>
       </c>
@@ -692,7 +692,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B12" s="3" t="s">
         <v>15</v>
       </c>
@@ -703,26 +703,26 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
         <v>26</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" t="s">
         <v>33</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -735,23 +735,23 @@
     <hyperlink ref="B5" r:id="rId6" xr:uid="{EBCE1FD2-6D15-4C0D-9A2D-FD93936B78DC}"/>
     <hyperlink ref="D2" r:id="rId7" xr:uid="{C6532461-6B4E-45AF-8A13-800522B4DB83}"/>
     <hyperlink ref="D3" r:id="rId8" xr:uid="{202382C4-0BCA-4431-AC77-9367E52A80AF}"/>
-    <hyperlink ref="D4" r:id="rId9" xr:uid="{08CAC529-6D21-45F2-A938-1E1042A85A0D}"/>
-    <hyperlink ref="D5" r:id="rId10" xr:uid="{339971EF-788C-4C51-9ACA-271F136B4960}"/>
-    <hyperlink ref="D6" r:id="rId11" xr:uid="{5947C907-21B9-4897-A6AB-A6CB74AC7CD5}"/>
-    <hyperlink ref="D7" r:id="rId12" xr:uid="{56BC170C-EB8A-4096-A6DB-28D20FF14F70}"/>
-    <hyperlink ref="B9" r:id="rId13" xr:uid="{C352C2CD-5FF1-4D94-BA71-6FE6B6FA64EC}"/>
-    <hyperlink ref="B10" r:id="rId14" xr:uid="{3066E82A-AAE5-49FB-B8AD-8E18257AF3F9}"/>
-    <hyperlink ref="B11" r:id="rId15" xr:uid="{0D901282-87C6-475F-A204-52ABD2ADC7A0}"/>
-    <hyperlink ref="B12" r:id="rId16" xr:uid="{41AF0875-636E-4A62-963B-72743FEB18B1}"/>
-    <hyperlink ref="D9" r:id="rId17" xr:uid="{37312FC1-399B-47D3-BA2E-71CDC7648070}"/>
-    <hyperlink ref="D10" r:id="rId18" xr:uid="{CF0FE52C-EA55-42AD-AF27-02D3F86A9172}"/>
-    <hyperlink ref="D12" r:id="rId19" xr:uid="{B50AA7AB-F016-40F2-8543-DA95B96F1044}"/>
-    <hyperlink ref="D11" r:id="rId20" xr:uid="{255CF652-B6DC-4FB3-A5D6-F681192DC6E6}"/>
-    <hyperlink ref="B13" r:id="rId21" xr:uid="{40D76F46-8BFB-416E-9171-5046520544EC}"/>
-    <hyperlink ref="D13" r:id="rId22" xr:uid="{C07EE079-CE56-4A08-9E96-6BC8B28404F7}"/>
-    <hyperlink ref="B8" r:id="rId23" xr:uid="{B616F6BF-5489-400E-9DF1-90D2894FCBBA}"/>
-    <hyperlink ref="D8" r:id="rId24" xr:uid="{15011053-4D3F-4C48-BDD3-84F60497BFFB}"/>
-    <hyperlink ref="D14" r:id="rId25" xr:uid="{3C40A261-9F64-4748-B069-ADB934FE4361}"/>
+    <hyperlink ref="D5" r:id="rId9" xr:uid="{339971EF-788C-4C51-9ACA-271F136B4960}"/>
+    <hyperlink ref="D6" r:id="rId10" xr:uid="{5947C907-21B9-4897-A6AB-A6CB74AC7CD5}"/>
+    <hyperlink ref="D7" r:id="rId11" xr:uid="{56BC170C-EB8A-4096-A6DB-28D20FF14F70}"/>
+    <hyperlink ref="B9" r:id="rId12" xr:uid="{C352C2CD-5FF1-4D94-BA71-6FE6B6FA64EC}"/>
+    <hyperlink ref="B10" r:id="rId13" xr:uid="{3066E82A-AAE5-49FB-B8AD-8E18257AF3F9}"/>
+    <hyperlink ref="B11" r:id="rId14" xr:uid="{0D901282-87C6-475F-A204-52ABD2ADC7A0}"/>
+    <hyperlink ref="B12" r:id="rId15" xr:uid="{41AF0875-636E-4A62-963B-72743FEB18B1}"/>
+    <hyperlink ref="D9" r:id="rId16" xr:uid="{37312FC1-399B-47D3-BA2E-71CDC7648070}"/>
+    <hyperlink ref="D10" r:id="rId17" xr:uid="{CF0FE52C-EA55-42AD-AF27-02D3F86A9172}"/>
+    <hyperlink ref="D12" r:id="rId18" xr:uid="{B50AA7AB-F016-40F2-8543-DA95B96F1044}"/>
+    <hyperlink ref="D11" r:id="rId19" xr:uid="{255CF652-B6DC-4FB3-A5D6-F681192DC6E6}"/>
+    <hyperlink ref="B13" r:id="rId20" xr:uid="{40D76F46-8BFB-416E-9171-5046520544EC}"/>
+    <hyperlink ref="D13" r:id="rId21" xr:uid="{C07EE079-CE56-4A08-9E96-6BC8B28404F7}"/>
+    <hyperlink ref="B8" r:id="rId22" xr:uid="{B616F6BF-5489-400E-9DF1-90D2894FCBBA}"/>
+    <hyperlink ref="D8" r:id="rId23" xr:uid="{15011053-4D3F-4C48-BDD3-84F60497BFFB}"/>
+    <hyperlink ref="D14" r:id="rId24" xr:uid="{3C40A261-9F64-4748-B069-ADB934FE4361}"/>
+    <hyperlink ref="D4" r:id="rId25" xr:uid="{0A2C3D29-09B6-B045-A331-AC95ECB5C110}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId26"/>
@@ -767,7 +767,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
@@ -782,7 +782,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>

</xml_diff>

<commit_message>
Added notes and deleted an app from the list
</commit_message>
<xml_diff>
--- a/Url_List.xlsx
+++ b/Url_List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://163gc-my.sharepoint.com/personal/abdelmonaam_kallali_ssc-spc_gc_ca/Documents/Documents/ProdApplicationMonitoring/ProdApplicationMonitoring/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="114_{E30C56CB-0642-486D-B1FB-CBD893529A96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0D26CF6E-7F60-F541-A4C8-FB127C80CFE9}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="114_{E30C56CB-0642-486D-B1FB-CBD893529A96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D5166978-9B91-324E-BCF2-1E02F0F6DC2C}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{D13659F6-ED47-4C0E-9560-3CD668E37EED}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16680" xr2:uid="{D13659F6-ED47-4C0E-9560-3CD668E37EED}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
   <si>
     <t>URL</t>
   </si>
@@ -85,9 +85,6 @@
     <t>https://atippal.ssc-spc.gc.ca</t>
   </si>
   <si>
-    <t>https://atippal-uat.ssc-spc.gc.ca</t>
-  </si>
-  <si>
     <t>ATIP</t>
   </si>
   <si>
@@ -95,9 +92,6 @@
   </si>
   <si>
     <t>ATIPPAL</t>
-  </si>
-  <si>
-    <t>ATIPPAL UAT</t>
   </si>
   <si>
     <t>https://Atip.ssc-spc.gc.ca/atipxpress</t>
@@ -558,10 +552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A17F301F-A4BC-4FEF-A93E-385FAF2DEAD9}">
-  <dimension ref="B1:D14"/>
+  <dimension ref="B1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -590,7 +584,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.2">
@@ -601,7 +595,7 @@
         <v>4</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.2">
@@ -612,7 +606,7 @@
         <v>11</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.2">
@@ -623,7 +617,7 @@
         <v>5</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.2">
@@ -634,7 +628,7 @@
         <v>7</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.2">
@@ -642,32 +636,32 @@
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="C9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.2">
@@ -675,54 +669,43 @@
         <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B11" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B12" s="3" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B13" s="3" t="s">
-        <v>25</v>
+      <c r="B13" t="s">
+        <v>30</v>
       </c>
       <c r="C13" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
         <v>32</v>
-      </c>
-      <c r="C14" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -741,20 +724,18 @@
     <hyperlink ref="B9" r:id="rId12" xr:uid="{C352C2CD-5FF1-4D94-BA71-6FE6B6FA64EC}"/>
     <hyperlink ref="B10" r:id="rId13" xr:uid="{3066E82A-AAE5-49FB-B8AD-8E18257AF3F9}"/>
     <hyperlink ref="B11" r:id="rId14" xr:uid="{0D901282-87C6-475F-A204-52ABD2ADC7A0}"/>
-    <hyperlink ref="B12" r:id="rId15" xr:uid="{41AF0875-636E-4A62-963B-72743FEB18B1}"/>
-    <hyperlink ref="D9" r:id="rId16" xr:uid="{37312FC1-399B-47D3-BA2E-71CDC7648070}"/>
-    <hyperlink ref="D10" r:id="rId17" xr:uid="{CF0FE52C-EA55-42AD-AF27-02D3F86A9172}"/>
-    <hyperlink ref="D12" r:id="rId18" xr:uid="{B50AA7AB-F016-40F2-8543-DA95B96F1044}"/>
-    <hyperlink ref="D11" r:id="rId19" xr:uid="{255CF652-B6DC-4FB3-A5D6-F681192DC6E6}"/>
-    <hyperlink ref="B13" r:id="rId20" xr:uid="{40D76F46-8BFB-416E-9171-5046520544EC}"/>
-    <hyperlink ref="D13" r:id="rId21" xr:uid="{C07EE079-CE56-4A08-9E96-6BC8B28404F7}"/>
-    <hyperlink ref="B8" r:id="rId22" xr:uid="{B616F6BF-5489-400E-9DF1-90D2894FCBBA}"/>
-    <hyperlink ref="D8" r:id="rId23" xr:uid="{15011053-4D3F-4C48-BDD3-84F60497BFFB}"/>
-    <hyperlink ref="D14" r:id="rId24" xr:uid="{3C40A261-9F64-4748-B069-ADB934FE4361}"/>
-    <hyperlink ref="D4" r:id="rId25" xr:uid="{0A2C3D29-09B6-B045-A331-AC95ECB5C110}"/>
+    <hyperlink ref="D9" r:id="rId15" xr:uid="{37312FC1-399B-47D3-BA2E-71CDC7648070}"/>
+    <hyperlink ref="D10" r:id="rId16" xr:uid="{CF0FE52C-EA55-42AD-AF27-02D3F86A9172}"/>
+    <hyperlink ref="D11" r:id="rId17" xr:uid="{255CF652-B6DC-4FB3-A5D6-F681192DC6E6}"/>
+    <hyperlink ref="B12" r:id="rId18" xr:uid="{40D76F46-8BFB-416E-9171-5046520544EC}"/>
+    <hyperlink ref="D12" r:id="rId19" xr:uid="{C07EE079-CE56-4A08-9E96-6BC8B28404F7}"/>
+    <hyperlink ref="B8" r:id="rId20" xr:uid="{B616F6BF-5489-400E-9DF1-90D2894FCBBA}"/>
+    <hyperlink ref="D8" r:id="rId21" xr:uid="{15011053-4D3F-4C48-BDD3-84F60497BFFB}"/>
+    <hyperlink ref="D13" r:id="rId22" xr:uid="{3C40A261-9F64-4748-B069-ADB934FE4361}"/>
+    <hyperlink ref="D4" r:id="rId23" xr:uid="{0A2C3D29-09B6-B045-A331-AC95ECB5C110}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId26"/>
+  <pageSetup orientation="portrait" r:id="rId24"/>
   <headerFooter>
     <oddHeader>&amp;R&amp;"Calibri"&amp;12&amp;K000000 Unclassified | Non classifié&amp;1#_x000D_</oddHeader>
   </headerFooter>

</xml_diff>

<commit_message>
removing Archer Dev from the list
</commit_message>
<xml_diff>
--- a/Url_List.xlsx
+++ b/Url_List.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://163gc-my.sharepoint.com/personal/abdelmonaam_kallali_ssc-spc_gc_ca/Documents/Documents/ProdApplicationMonitoring/ProdApplicationMonitoring/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="114_{E30C56CB-0642-486D-B1FB-CBD893529A96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D5166978-9B91-324E-BCF2-1E02F0F6DC2C}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="114_{E30C56CB-0642-486D-B1FB-CBD893529A96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{29EE583B-FF8F-5546-941D-DE172A7C56ED}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16680" xr2:uid="{D13659F6-ED47-4C0E-9560-3CD668E37EED}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
   <si>
     <t>URL</t>
   </si>
@@ -71,12 +71,6 @@
   </si>
   <si>
     <t>https://reservation.ssc-spc.gc.ca/archibus/schema/ab-products/essential/workplace/</t>
-  </si>
-  <si>
-    <t>Archer Dev</t>
-  </si>
-  <si>
-    <t>https://archer-dev.ssc-spc.gc.ca/RSAarcher</t>
   </si>
   <si>
     <t>Email</t>
@@ -253,6 +247,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -552,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A17F301F-A4BC-4FEF-A93E-385FAF2DEAD9}">
-  <dimension ref="B1:D13"/>
+  <dimension ref="B1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD12"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -573,7 +571,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.2">
@@ -584,7 +582,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.2">
@@ -595,147 +593,134 @@
         <v>4</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B4" s="3" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="C7" t="s">
         <v>26</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B9" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
         <v>15</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s">
         <v>14</v>
       </c>
-      <c r="C10" t="s">
-        <v>17</v>
-      </c>
       <c r="D10" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B11" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B12" s="3" t="s">
-        <v>23</v>
+      <c r="B12" t="s">
+        <v>28</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
         <v>30</v>
-      </c>
-      <c r="C13" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{7D113961-7C60-48BC-BC8F-E6D2F65EC94E}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{302FFEA7-2C43-4709-BB3F-C79D63957060}"/>
-    <hyperlink ref="B6" r:id="rId3" xr:uid="{C6681F13-9568-4EFE-A59B-8A109A7A7A08}"/>
-    <hyperlink ref="B7" r:id="rId4" xr:uid="{DD3DA419-5FFB-4B94-882D-76CD30B15763}"/>
-    <hyperlink ref="B4" r:id="rId5" xr:uid="{38A7B278-C43A-405C-A6CE-5EAB7A3CFF8F}"/>
-    <hyperlink ref="B5" r:id="rId6" xr:uid="{EBCE1FD2-6D15-4C0D-9A2D-FD93936B78DC}"/>
-    <hyperlink ref="D2" r:id="rId7" xr:uid="{C6532461-6B4E-45AF-8A13-800522B4DB83}"/>
-    <hyperlink ref="D3" r:id="rId8" xr:uid="{202382C4-0BCA-4431-AC77-9367E52A80AF}"/>
-    <hyperlink ref="D5" r:id="rId9" xr:uid="{339971EF-788C-4C51-9ACA-271F136B4960}"/>
-    <hyperlink ref="D6" r:id="rId10" xr:uid="{5947C907-21B9-4897-A6AB-A6CB74AC7CD5}"/>
-    <hyperlink ref="D7" r:id="rId11" xr:uid="{56BC170C-EB8A-4096-A6DB-28D20FF14F70}"/>
-    <hyperlink ref="B9" r:id="rId12" xr:uid="{C352C2CD-5FF1-4D94-BA71-6FE6B6FA64EC}"/>
-    <hyperlink ref="B10" r:id="rId13" xr:uid="{3066E82A-AAE5-49FB-B8AD-8E18257AF3F9}"/>
-    <hyperlink ref="B11" r:id="rId14" xr:uid="{0D901282-87C6-475F-A204-52ABD2ADC7A0}"/>
-    <hyperlink ref="D9" r:id="rId15" xr:uid="{37312FC1-399B-47D3-BA2E-71CDC7648070}"/>
-    <hyperlink ref="D10" r:id="rId16" xr:uid="{CF0FE52C-EA55-42AD-AF27-02D3F86A9172}"/>
-    <hyperlink ref="D11" r:id="rId17" xr:uid="{255CF652-B6DC-4FB3-A5D6-F681192DC6E6}"/>
-    <hyperlink ref="B12" r:id="rId18" xr:uid="{40D76F46-8BFB-416E-9171-5046520544EC}"/>
-    <hyperlink ref="D12" r:id="rId19" xr:uid="{C07EE079-CE56-4A08-9E96-6BC8B28404F7}"/>
-    <hyperlink ref="B8" r:id="rId20" xr:uid="{B616F6BF-5489-400E-9DF1-90D2894FCBBA}"/>
-    <hyperlink ref="D8" r:id="rId21" xr:uid="{15011053-4D3F-4C48-BDD3-84F60497BFFB}"/>
-    <hyperlink ref="D13" r:id="rId22" xr:uid="{3C40A261-9F64-4748-B069-ADB934FE4361}"/>
-    <hyperlink ref="D4" r:id="rId23" xr:uid="{0A2C3D29-09B6-B045-A331-AC95ECB5C110}"/>
+    <hyperlink ref="B5" r:id="rId3" xr:uid="{C6681F13-9568-4EFE-A59B-8A109A7A7A08}"/>
+    <hyperlink ref="B6" r:id="rId4" xr:uid="{DD3DA419-5FFB-4B94-882D-76CD30B15763}"/>
+    <hyperlink ref="B4" r:id="rId5" xr:uid="{EBCE1FD2-6D15-4C0D-9A2D-FD93936B78DC}"/>
+    <hyperlink ref="D2" r:id="rId6" xr:uid="{C6532461-6B4E-45AF-8A13-800522B4DB83}"/>
+    <hyperlink ref="D3" r:id="rId7" xr:uid="{202382C4-0BCA-4431-AC77-9367E52A80AF}"/>
+    <hyperlink ref="D4" r:id="rId8" xr:uid="{339971EF-788C-4C51-9ACA-271F136B4960}"/>
+    <hyperlink ref="D5" r:id="rId9" xr:uid="{5947C907-21B9-4897-A6AB-A6CB74AC7CD5}"/>
+    <hyperlink ref="D6" r:id="rId10" xr:uid="{56BC170C-EB8A-4096-A6DB-28D20FF14F70}"/>
+    <hyperlink ref="B8" r:id="rId11" xr:uid="{C352C2CD-5FF1-4D94-BA71-6FE6B6FA64EC}"/>
+    <hyperlink ref="B9" r:id="rId12" xr:uid="{3066E82A-AAE5-49FB-B8AD-8E18257AF3F9}"/>
+    <hyperlink ref="B10" r:id="rId13" xr:uid="{0D901282-87C6-475F-A204-52ABD2ADC7A0}"/>
+    <hyperlink ref="D8" r:id="rId14" xr:uid="{37312FC1-399B-47D3-BA2E-71CDC7648070}"/>
+    <hyperlink ref="D9" r:id="rId15" xr:uid="{CF0FE52C-EA55-42AD-AF27-02D3F86A9172}"/>
+    <hyperlink ref="D10" r:id="rId16" xr:uid="{255CF652-B6DC-4FB3-A5D6-F681192DC6E6}"/>
+    <hyperlink ref="B11" r:id="rId17" xr:uid="{40D76F46-8BFB-416E-9171-5046520544EC}"/>
+    <hyperlink ref="D11" r:id="rId18" xr:uid="{C07EE079-CE56-4A08-9E96-6BC8B28404F7}"/>
+    <hyperlink ref="B7" r:id="rId19" xr:uid="{B616F6BF-5489-400E-9DF1-90D2894FCBBA}"/>
+    <hyperlink ref="D7" r:id="rId20" xr:uid="{15011053-4D3F-4C48-BDD3-84F60497BFFB}"/>
+    <hyperlink ref="D12" r:id="rId21" xr:uid="{3C40A261-9F64-4748-B069-ADB934FE4361}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId24"/>
+  <pageSetup orientation="portrait" r:id="rId22"/>
   <headerFooter>
     <oddHeader>&amp;R&amp;"Calibri"&amp;12&amp;K000000 Unclassified | Non classifié&amp;1#_x000D_</oddHeader>
   </headerFooter>

</xml_diff>

<commit_message>
Update Cira to SSC360 and added email
</commit_message>
<xml_diff>
--- a/Url_List.xlsx
+++ b/Url_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LoweS2\Desktop\test\ProdApplicationMonitoring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22BB9487-7592-4DED-9CD3-B7E852A7FD1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{276132F6-6737-42E0-A6F1-15BA7BBC6FB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -52,9 +52,6 @@
     <t>https://sscpp-ppspc.crm3.dynamics.com/</t>
   </si>
   <si>
-    <t>Justine.Eisenhour@ssc-spc.gc.ca,ssc.ppcoesupport-cdeppsupport.spc@ssc-spc.gc.ca</t>
-  </si>
-  <si>
     <t>https://plus.ssc-spc.gc.ca/en</t>
   </si>
   <si>
@@ -116,13 +113,16 @@
   </si>
   <si>
     <t>SSC360</t>
+  </si>
+  <si>
+    <t>Justine.Eisenhour@ssc-spc.gc.ca,ssc.ppcoesupport-cdeppsupport.spc@ssc-spc.gc.ca,najet.nouisser@ssc-spc.gc.ca</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -134,6 +134,14 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -168,16 +176,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -481,13 +492,14 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="61.7109375" customWidth="1"/>
     <col min="3" max="3" width="33.85546875" customWidth="1"/>
+    <col min="4" max="4" width="156.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -529,101 +541,104 @@
         <v>9</v>
       </c>
       <c r="C4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
         <v>11</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>12</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
         <v>14</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>15</v>
-      </c>
-      <c r="D6" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
         <v>17</v>
       </c>
-      <c r="C7" t="s">
-        <v>18</v>
-      </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
         <v>19</v>
       </c>
-      <c r="C8" t="s">
-        <v>20</v>
-      </c>
       <c r="D8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
         <v>21</v>
       </c>
-      <c r="C9" t="s">
-        <v>22</v>
-      </c>
       <c r="D9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
         <v>23</v>
       </c>
-      <c r="C10" t="s">
-        <v>24</v>
-      </c>
       <c r="D10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
         <v>25</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>26</v>
-      </c>
-      <c r="D11" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" t="s">
         <v>28</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>29</v>
       </c>
-      <c r="D12" t="s">
-        <v>30</v>
-      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D4" r:id="rId1" xr:uid="{4773560E-489E-4341-A9BB-00CCCCEF883B}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter>
     <oddHeader>&amp;R&amp;"Calibri"&amp;12&amp;K000000 Unclassified | Non classifié&amp;1#_x000D_</oddHeader>

</xml_diff>

<commit_message>
Updated URL for SSC360
</commit_message>
<xml_diff>
--- a/Url_List.xlsx
+++ b/Url_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LoweS2\Desktop\test\ProdApplicationMonitoring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{276132F6-6737-42E0-A6F1-15BA7BBC6FB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0061020-899A-414A-B169-5307765A96CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,9 +49,6 @@
     <t>abdelmonaam.kallali@ssc-spc.gc.ca,abdellah.arba@ssc-spc.gc.ca,archermanagement-gestiondearcher@ssc-spc.gc.ca</t>
   </si>
   <si>
-    <t>https://sscpp-ppspc.crm3.dynamics.com/</t>
-  </si>
-  <si>
     <t>https://plus.ssc-spc.gc.ca/en</t>
   </si>
   <si>
@@ -116,6 +113,9 @@
   </si>
   <si>
     <t>Justine.Eisenhour@ssc-spc.gc.ca,ssc.ppcoesupport-cdeppsupport.spc@ssc-spc.gc.ca,najet.nouisser@ssc-spc.gc.ca</t>
+  </si>
+  <si>
+    <t>https://sscpp-ppspc-360-ent.crm3.dynamics.com/</t>
   </si>
 </sst>
 </file>
@@ -492,12 +492,12 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="61.7109375" customWidth="1"/>
+    <col min="2" max="2" width="90" customWidth="1"/>
     <col min="3" max="3" width="33.85546875" customWidth="1"/>
     <col min="4" max="4" width="156.42578125" customWidth="1"/>
   </cols>
@@ -537,107 +537,108 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>9</v>
+      <c r="B4" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="C4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>11</v>
-      </c>
-      <c r="D5" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
         <v>13</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>14</v>
-      </c>
-      <c r="D6" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
         <v>16</v>
       </c>
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
         <v>18</v>
       </c>
-      <c r="C8" t="s">
-        <v>19</v>
-      </c>
       <c r="D8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
         <v>20</v>
       </c>
-      <c r="C9" t="s">
-        <v>21</v>
-      </c>
       <c r="D9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" t="s">
         <v>22</v>
       </c>
-      <c r="C10" t="s">
-        <v>23</v>
-      </c>
       <c r="D10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
         <v>24</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>25</v>
-      </c>
-      <c r="D11" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" t="s">
         <v>27</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>28</v>
-      </c>
-      <c r="D12" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D4" r:id="rId1" xr:uid="{4773560E-489E-4341-A9BB-00CCCCEF883B}"/>
+    <hyperlink ref="B4" r:id="rId2" tooltip="https://sscpp-ppspc-360-ent.crm3.dynamics.com/" xr:uid="{235148D9-5D52-45A1-9A20-273595CF8553}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter>

</xml_diff>